<commit_message>
Update profit files after running on 2025-11-27
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,40 @@
         <v>-17.99</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>11/27/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15267.71</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1556293945131625</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.8443706054868375</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-33.25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-8.640000000000001</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-17550.15</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-57.65</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-376.75</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-13.69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-28
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,40 @@
         <v>-13.69</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>11/28/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>14420.48</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1652883499150231</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8347116500849769</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-58.58</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-14.29</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-18429.81</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-60.49</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-369.31</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-13.42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-29
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,40 @@
         <v>-13.42</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11/29/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>14475.31</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1631502794106506</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8368497205893494</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-56.34</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-13.74</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-18353.1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-60.24</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-391.2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-14.21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-11-30
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,6 +621,40 @@
         <v>-14.21</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11/30/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>14780.29</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1573518266434222</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8426481733565778</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-46.38</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-11.31</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-18012.17</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-59.12</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-477.14</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-17.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-01
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,6 +655,40 @@
         <v>-17.02</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12/01/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>12960.19</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1667601265990996</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8332398734009004</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-94.72</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-23.1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-19667.81</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-64.55</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-641.61</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-22.89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-02
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,6 +689,40 @@
         <v>-22.89</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12/02/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>13588.87</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.163755904415552</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.836244095584448</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-78.23</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-19.08</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-19103.15</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-62.7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-577.59</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-20.61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-03
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,6 +723,40 @@
         <v>-20.61</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>12/03/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14460.2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.163896978737768</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.836103021262232</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-57.02</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-13.91</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-18376.54</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-60.32</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-432.87</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-15.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-04
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,6 +757,40 @@
         <v>-15.44</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>12/04/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>14644.2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.162034656703162</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.837965343296838</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-51.73</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-12.62</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-18195.42</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-59.72</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-429.98</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-15.34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-05
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,40 @@
         <v>-15.34</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>12/05/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>13733.35</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1692956467811615</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8307043532188385</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-76.93000000000001</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-18.76</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-19058.4</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-62.55</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-477.85</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-17.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-06
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,6 +825,40 @@
         <v>-17.05</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>12/06/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>13382.72</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.1706518523656737</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8293481476343263</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-88.65000000000001</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-20.38</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-19392.82</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-63.6</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-519.0599999999999</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-18.52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-07
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,6 +859,40 @@
         <v>-18.52</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12/07/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>13193.07</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1724867103395756</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.8275132896604244</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-94.31</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-21.68</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-19574.32</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-64.2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-527.22</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-18.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-08
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,6 +893,40 @@
         <v>-18.81</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>12/08/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13633.28</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.171641667611514</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.828358332388486</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-82.58</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-18.98</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-19198.52</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-62.96</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-462.81</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-16.51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-09
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -927,6 +927,40 @@
         <v>-16.51</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>12/09/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>13162.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1905027776609068</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.8094972223390932</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-102.51</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-23.57</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-19836.95</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-65.06</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-395.4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-13.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-10
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,6 +961,40 @@
         <v>-13.62</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>12/10/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>13219.05</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.1922042298597978</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8077957701402022</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-101.77</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-23.4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-19813.46</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-64.98</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-362.09</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-12.47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-11
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,6 +995,40 @@
         <v>-12.47</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>12/11/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>12749.24</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.1957653634455948</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8042346365544052</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-115.03</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-26.44</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-20238.37</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-66.37</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-406.99</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-14.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-12
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,6 +1029,40 @@
         <v>-14.02</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>12/12/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>12589.72</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.2026587542587263</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.7973412457412737</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-123.43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-26.83</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-20478.46</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-67.11</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-351.43</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-12.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-13
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1063,6 +1063,40 @@
         <v>-12.11</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>12/13/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>12398.31</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2015704448859508</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.7984295551140492</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-128.1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-27.85</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-20617.58</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-67.56</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-403.72</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-13.91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-14
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1097,6 +1097,40 @@
         <v>-13.91</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>12/14/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>12298.94</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.2055609289118182</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.7944390710881818</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-132.4</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-28.78</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-20746</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-67.98</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-424.67</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-14.38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-15
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1131,6 +1131,40 @@
         <v>-14.38</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>12/15/2025</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>12063.13</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.2097260978964278</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.7902739021035722</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-140.37</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-30.52</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-20983.58</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-68.76000000000001</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-422.9</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-14.32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-16
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,6 +1165,40 @@
         <v>-14.32</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>12/16/2025</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>11757.73</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.2092236483795707</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.7907763516204293</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-148.26</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-32.23</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-21219.02</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-69.53</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-492.85</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-16.69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-17
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1199,6 +1199,40 @@
         <v>-16.69</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>12/17/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>11777.44</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.20854811384464</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.79145188615536</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-147.47</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-32.06</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-21195.48</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-69.45999999999999</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-496.69</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-16.82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-18
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,6 +1233,40 @@
         <v>-16.82</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>12/18/2025</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>11475.31</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.2143824212507974</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.7856175787492026</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-157.74</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-34.29</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-21501.55</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-70.45999999999999</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-492.74</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-16.69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-19
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1267,6 +1267,40 @@
         <v>-16.69</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>12/19/2025</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>11621.65</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.2137860489086395</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.7862139510913605</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-153.93</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-31.74</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-21404.65</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-70.08</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-468.3</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-15.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-20
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1301,6 +1301,40 @@
         <v>-15.86</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>12/20/2025</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12040.8</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.206572700787405</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.793427299212595</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-138.84</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-28.63</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-20988.26</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-68.72</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-465.55</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-15.77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-21
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,6 +1335,40 @@
         <v>-15.77</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>12/21/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>12382.38</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.2059261044743488</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.7940738955256512</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-128.73</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-26.54</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-20709.23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-67.81</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-452.99</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-15.09</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-22
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1369,6 +1369,40 @@
         <v>-15.09</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12/22/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>13002.96</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.1994203710065661</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.8005796289934339</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-107.81</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-22.23</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-20131.86</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-65.92</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-409.8</v>
+      </c>
+      <c r="J28" t="n">
+        <v>-13.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-23
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1403,6 +1403,40 @@
         <v>-13.65</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>12/23/2025</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>12280.2</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.2057852427978976</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.7942147572021024</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-131.61</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-27.14</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-20788.65</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-68.06999999999999</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-475.77</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-15.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-24
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,6 +1437,40 @@
         <v>-15.84</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12/24/2025</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>12129.23</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.2070483707744404</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.7929516292255596</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-136.51</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-28.15</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-20923.87</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-68.51000000000001</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-491.51</v>
+      </c>
+      <c r="J30" t="n">
+        <v>-16.37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-25
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1471,6 +1471,40 @@
         <v>-16.37</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>12/25/2025</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>12014.72</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.209495172465466</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.790504827534534</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-140.86</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-29.04</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-21044.06</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-68.90000000000001</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-485.82</v>
+      </c>
+      <c r="J31" t="n">
+        <v>-16.18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-26
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1505,6 +1505,40 @@
         <v>-16.18</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12/26/2025</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>12401.14</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.205772699318881</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.794227300681119</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-128.84</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-24.08</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-20742.43</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-67.8</v>
+      </c>
+      <c r="I32" t="n">
+        <v>-451.03</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-15.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-27
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1539,6 +1539,40 @@
         <v>-15.02</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12/27/2025</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>12167.42</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.206830545967442</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.793169454032558</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-137.02</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-25.61</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-20940.93</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-68.45</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-486.26</v>
+      </c>
+      <c r="J33" t="n">
+        <v>-16.19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-28
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1573,6 +1573,40 @@
         <v>-16.19</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>12/28/2025</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>12175.48</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.21143141114929</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.78856858885071</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-139.07</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-25.99</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-20990.56</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-68.62</v>
+      </c>
+      <c r="I34" t="n">
+        <v>-478.57</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-15.68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-29
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1607,6 +1607,40 @@
         <v>-15.68</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>12/29/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>12063.57</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.212164207900799</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.787835792099201</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-143.07</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-26.74</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-21087.65</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-68.93000000000001</v>
+      </c>
+      <c r="I35" t="n">
+        <v>-493.39</v>
+      </c>
+      <c r="J35" t="n">
+        <v>-16.16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-30
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1641,6 +1641,40 @@
         <v>-16.16</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>12/30/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>11954</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.2155915824299713</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.7844084175700287</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-148.32</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-27.72</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-21214.94</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-69.34999999999999</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-475.67</v>
+      </c>
+      <c r="J36" t="n">
+        <v>-15.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2025-12-31
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1675,6 +1675,40 @@
         <v>-15.58</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>12/31/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>12081.49</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.2154755965780969</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.7845244034219031</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-144.14</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-26.94</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-21113.54</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-69.02</v>
+      </c>
+      <c r="I37" t="n">
+        <v>-449.58</v>
+      </c>
+      <c r="J37" t="n">
+        <v>-14.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-01
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1709,6 +1709,40 @@
         <v>-14.73</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>11770.23</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.2189261117235364</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.7810738882764636</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-155.88</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-29.14</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-21398.34</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-69.95</v>
+      </c>
+      <c r="I38" t="n">
+        <v>-476.04</v>
+      </c>
+      <c r="J38" t="n">
+        <v>-15.59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-02
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1743,6 +1743,40 @@
         <v>-15.59</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>12417.46</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.2113242502079662</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.7886757497920338</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-133.45</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-22.81</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-20848.41</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-68.04000000000001</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-428.74</v>
+      </c>
+      <c r="J39" t="n">
+        <v>-14.04</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-03
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1777,6 +1777,40 @@
         <v>-14.04</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>01/03/2026</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>12284.42</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.2142576612486495</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.7857423387513505</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-139.95</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-23.92</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-20989.37</v>
+      </c>
+      <c r="H40" t="n">
+        <v>-68.5</v>
+      </c>
+      <c r="I40" t="n">
+        <v>-420.82</v>
+      </c>
+      <c r="J40" t="n">
+        <v>-13.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-04
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1811,6 +1811,40 @@
         <v>-13.78</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>01/04/2026</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>13302.26</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.2046055683399551</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.7953944316600449</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-97.15000000000001</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-16.61</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-20061.21</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-65.47</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-381.13</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-12.28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-05
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1845,6 +1845,40 @@
         <v>-12.28</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>01/05/2026</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>13601.81</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.2037872448926116</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.7962127551073884</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-85.65000000000001</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-14.64</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-19811.82</v>
+      </c>
+      <c r="H42" t="n">
+        <v>-64.66</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-331.24</v>
+      </c>
+      <c r="J42" t="n">
+        <v>-10.68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-06
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1879,6 +1879,40 @@
         <v>-10.68</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>01/06/2026</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>14307.32</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.1959103068579821</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.8040896931420179</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-54.56</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-9.33</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-19137.39</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-62.46</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-299.9</v>
+      </c>
+      <c r="J43" t="n">
+        <v>-9.67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-07
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1913,6 +1913,40 @@
         <v>-9.67</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>01/07/2026</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>13553.9</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.2027326824535619</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.7972673175464381</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-86.75</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-14.83</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-19835.68</v>
+      </c>
+      <c r="H44" t="n">
+        <v>-64.73</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-355.03</v>
+      </c>
+      <c r="J44" t="n">
+        <v>-11.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-08
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1947,6 +1947,40 @@
         <v>-11.44</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>01/08/2026</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>12635.58</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.2125815996498773</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.7874184003501227</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-126.25</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-21.58</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-20692.27</v>
+      </c>
+      <c r="H45" t="n">
+        <v>-67.53</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-416.76</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-13.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-09
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1981,6 +1981,40 @@
         <v>-13.43</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>01/09/2026</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>12871.43</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.2097603367030337</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.7902396632969663</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-119.71</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-18.85</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-20520.24</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-66.86</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-402.93</v>
+      </c>
+      <c r="J46" t="n">
+        <v>-12.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-10
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2015,6 +2015,40 @@
         <v>-12.99</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>01/10/2026</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>12897.3</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.2098245391966422</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.7901754608033578</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-118.72</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-18.7</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-20500.63</v>
+      </c>
+      <c r="H47" t="n">
+        <v>-66.8</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-396.68</v>
+      </c>
+      <c r="J47" t="n">
+        <v>-12.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-11
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2049,6 +2049,40 @@
         <v>-12.78</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>01/11/2026</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>13216.22</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.2091078640570865</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.7908921359429135</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-105.47</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-16.61</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-20239.15</v>
+      </c>
+      <c r="H48" t="n">
+        <v>-65.94</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-389.23</v>
+      </c>
+      <c r="J48" t="n">
+        <v>-12.35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-12
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2083,6 +2083,40 @@
         <v>-12.35</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>01/12/2026</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>12844.42</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.2147146019633982</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.7852853980366018</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-124.01</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-19.53</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-20605.22</v>
+      </c>
+      <c r="H49" t="n">
+        <v>-67.14</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-394.97</v>
+      </c>
+      <c r="J49" t="n">
+        <v>-12.53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-13
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2117,6 +2117,40 @@
         <v>-12.53</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>01/13/2026</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>13182.45</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.2123713965796088</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.7876286034203912</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-109</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-17.17</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-20308.88</v>
+      </c>
+      <c r="H50" t="n">
+        <v>-66.17</v>
+      </c>
+      <c r="I50" t="n">
+        <v>-353.27</v>
+      </c>
+      <c r="J50" t="n">
+        <v>-11.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-14
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2151,6 +2151,40 @@
         <v>-11.2</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>01/14/2026</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>13305.92</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.2172232585151117</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.7827767414848883</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-107.35</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-16.91</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-20276.2</v>
+      </c>
+      <c r="H51" t="n">
+        <v>-66.06</v>
+      </c>
+      <c r="I51" t="n">
+        <v>-262.5</v>
+      </c>
+      <c r="J51" t="n">
+        <v>-8.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-15
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,6 +2185,40 @@
         <v>-8.33</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>01/15/2026</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>13219.41</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.222814822013932</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.777185177986068</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-114.52</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-18.03</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-20417.83</v>
+      </c>
+      <c r="H52" t="n">
+        <v>-66.53</v>
+      </c>
+      <c r="I52" t="n">
+        <v>-207.37</v>
+      </c>
+      <c r="J52" t="n">
+        <v>-6.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-16
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>BTC Profit(%)</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Combined Total Profit(USD)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Combined Total Profit(%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -518,6 +528,8 @@
       <c r="J2" t="n">
         <v>-17.99</v>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -552,6 +564,8 @@
       <c r="J3" t="n">
         <v>-13.69</v>
       </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -586,6 +600,8 @@
       <c r="J4" t="n">
         <v>-13.42</v>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -620,6 +636,8 @@
       <c r="J5" t="n">
         <v>-14.21</v>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -654,6 +672,8 @@
       <c r="J6" t="n">
         <v>-17.02</v>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -688,6 +708,8 @@
       <c r="J7" t="n">
         <v>-22.89</v>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -722,6 +744,8 @@
       <c r="J8" t="n">
         <v>-20.61</v>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -756,6 +780,8 @@
       <c r="J9" t="n">
         <v>-15.44</v>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -790,6 +816,8 @@
       <c r="J10" t="n">
         <v>-15.34</v>
       </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -824,6 +852,8 @@
       <c r="J11" t="n">
         <v>-17.05</v>
       </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -858,6 +888,8 @@
       <c r="J12" t="n">
         <v>-18.52</v>
       </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -892,6 +924,8 @@
       <c r="J13" t="n">
         <v>-18.81</v>
       </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -926,6 +960,8 @@
       <c r="J14" t="n">
         <v>-16.51</v>
       </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -960,6 +996,8 @@
       <c r="J15" t="n">
         <v>-13.62</v>
       </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -994,6 +1032,8 @@
       <c r="J16" t="n">
         <v>-12.47</v>
       </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1028,6 +1068,8 @@
       <c r="J17" t="n">
         <v>-14.02</v>
       </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1062,6 +1104,8 @@
       <c r="J18" t="n">
         <v>-12.11</v>
       </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1096,6 +1140,8 @@
       <c r="J19" t="n">
         <v>-13.91</v>
       </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1130,6 +1176,8 @@
       <c r="J20" t="n">
         <v>-14.38</v>
       </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1164,6 +1212,8 @@
       <c r="J21" t="n">
         <v>-14.32</v>
       </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1198,6 +1248,8 @@
       <c r="J22" t="n">
         <v>-16.69</v>
       </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1232,6 +1284,8 @@
       <c r="J23" t="n">
         <v>-16.82</v>
       </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1266,6 +1320,8 @@
       <c r="J24" t="n">
         <v>-16.69</v>
       </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1300,6 +1356,8 @@
       <c r="J25" t="n">
         <v>-15.86</v>
       </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1334,6 +1392,8 @@
       <c r="J26" t="n">
         <v>-15.77</v>
       </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1368,6 +1428,8 @@
       <c r="J27" t="n">
         <v>-15.09</v>
       </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1402,6 +1464,8 @@
       <c r="J28" t="n">
         <v>-13.65</v>
       </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1436,6 +1500,8 @@
       <c r="J29" t="n">
         <v>-15.84</v>
       </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1470,6 +1536,8 @@
       <c r="J30" t="n">
         <v>-16.37</v>
       </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1504,6 +1572,8 @@
       <c r="J31" t="n">
         <v>-16.18</v>
       </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1538,6 +1608,8 @@
       <c r="J32" t="n">
         <v>-15.02</v>
       </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1572,6 +1644,8 @@
       <c r="J33" t="n">
         <v>-16.19</v>
       </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1606,6 +1680,8 @@
       <c r="J34" t="n">
         <v>-15.68</v>
       </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1640,6 +1716,8 @@
       <c r="J35" t="n">
         <v>-16.16</v>
       </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1674,6 +1752,8 @@
       <c r="J36" t="n">
         <v>-15.58</v>
       </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1708,6 +1788,8 @@
       <c r="J37" t="n">
         <v>-14.73</v>
       </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1742,6 +1824,8 @@
       <c r="J38" t="n">
         <v>-15.59</v>
       </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1776,6 +1860,8 @@
       <c r="J39" t="n">
         <v>-14.04</v>
       </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1810,6 +1896,8 @@
       <c r="J40" t="n">
         <v>-13.78</v>
       </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1844,6 +1932,8 @@
       <c r="J41" t="n">
         <v>-12.28</v>
       </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1878,6 +1968,8 @@
       <c r="J42" t="n">
         <v>-10.68</v>
       </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1912,6 +2004,8 @@
       <c r="J43" t="n">
         <v>-9.67</v>
       </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1946,6 +2040,8 @@
       <c r="J44" t="n">
         <v>-11.44</v>
       </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1980,6 +2076,8 @@
       <c r="J45" t="n">
         <v>-13.43</v>
       </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2014,6 +2112,8 @@
       <c r="J46" t="n">
         <v>-12.99</v>
       </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2048,6 +2148,8 @@
       <c r="J47" t="n">
         <v>-12.78</v>
       </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2082,6 +2184,8 @@
       <c r="J48" t="n">
         <v>-12.35</v>
       </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2116,6 +2220,8 @@
       <c r="J49" t="n">
         <v>-12.53</v>
       </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2150,6 +2256,8 @@
       <c r="J50" t="n">
         <v>-11.2</v>
       </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2184,6 +2292,8 @@
       <c r="J51" t="n">
         <v>-8.33</v>
       </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2217,6 +2327,48 @@
       </c>
       <c r="J52" t="n">
         <v>-6.58</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>01/16/2026</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>12796.09</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.2266795759358105</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.7733204240641895</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-137.53</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-20.08</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-20846.28</v>
+      </c>
+      <c r="H53" t="n">
+        <v>-67.81</v>
+      </c>
+      <c r="I53" t="n">
+        <v>-252.24</v>
+      </c>
+      <c r="J53" t="n">
+        <v>-8</v>
+      </c>
+      <c r="K53" t="n">
+        <v>-21098.52</v>
+      </c>
+      <c r="L53" t="n">
+        <v>-62.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-17
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2371,6 +2371,46 @@
         <v>-62.25</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>01/17/2026</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>12724.3</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.22765093445746</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.77234906554254</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-141.28</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-20.62</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-20914.16</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-68.03</v>
+      </c>
+      <c r="I54" t="n">
+        <v>-256.15</v>
+      </c>
+      <c r="J54" t="n">
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="K54" t="n">
+        <v>-21170.31</v>
+      </c>
+      <c r="L54" t="n">
+        <v>-62.46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-18
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2411,6 +2411,46 @@
         <v>-62.46</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>01/18/2026</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>12566.24</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.2341426964151604</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.7658573035848396</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-152.55</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-22.27</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-21117.81</v>
+      </c>
+      <c r="H55" t="n">
+        <v>-68.69</v>
+      </c>
+      <c r="I55" t="n">
+        <v>-260.56</v>
+      </c>
+      <c r="J55" t="n">
+        <v>-8.140000000000001</v>
+      </c>
+      <c r="K55" t="n">
+        <v>-21378.37</v>
+      </c>
+      <c r="L55" t="n">
+        <v>-62.98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-19
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2451,6 +2451,46 @@
         <v>-62.98</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>01/19/2026</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>12275.14</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.2343547161733963</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.7656452838266037</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-165.03</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-24.09</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-21343.35</v>
+      </c>
+      <c r="H56" t="n">
+        <v>-69.43000000000001</v>
+      </c>
+      <c r="I56" t="n">
+        <v>-326.11</v>
+      </c>
+      <c r="J56" t="n">
+        <v>-10.18</v>
+      </c>
+      <c r="K56" t="n">
+        <v>-21669.46</v>
+      </c>
+      <c r="L56" t="n">
+        <v>-63.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-20
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2491,6 +2491,46 @@
         <v>-63.84</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>01/20/2026</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>11973.81</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.2355691143938523</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.7644308856061477</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-178.59</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-26.07</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-21588.6</v>
+      </c>
+      <c r="H57" t="n">
+        <v>-70.23</v>
+      </c>
+      <c r="I57" t="n">
+        <v>-382.19</v>
+      </c>
+      <c r="J57" t="n">
+        <v>-11.93</v>
+      </c>
+      <c r="K57" t="n">
+        <v>-21970.79</v>
+      </c>
+      <c r="L57" t="n">
+        <v>-64.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-21
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2531,6 +2531,46 @@
         <v>-64.73</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>01/21/2026</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>11599.77</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.236403919765626</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.763596080234374</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-194.95</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-28.46</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-21884.22</v>
+      </c>
+      <c r="H58" t="n">
+        <v>-71.19</v>
+      </c>
+      <c r="I58" t="n">
+        <v>-460.62</v>
+      </c>
+      <c r="J58" t="n">
+        <v>-14.38</v>
+      </c>
+      <c r="K58" t="n">
+        <v>-22344.84</v>
+      </c>
+      <c r="L58" t="n">
+        <v>-65.83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-22
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2571,6 +2571,46 @@
         <v>-65.83</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>01/22/2026</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>11667.46</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.2383940354361063</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.7616059645638937</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-193.38</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-28.23</v>
+      </c>
+      <c r="G59" t="n">
+        <v>-21855.75</v>
+      </c>
+      <c r="H59" t="n">
+        <v>-71.09</v>
+      </c>
+      <c r="I59" t="n">
+        <v>-421.4</v>
+      </c>
+      <c r="J59" t="n">
+        <v>-13.16</v>
+      </c>
+      <c r="K59" t="n">
+        <v>-22277.15</v>
+      </c>
+      <c r="L59" t="n">
+        <v>-65.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-23
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2611,6 +2611,46 @@
         <v>-65.63</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>01/23/2026</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>11548.83</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.2389776229415066</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.7610223770584934</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-206</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-28.03</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-22002.84</v>
+      </c>
+      <c r="H60" t="n">
+        <v>-71.45999999999999</v>
+      </c>
+      <c r="I60" t="n">
+        <v>-442.94</v>
+      </c>
+      <c r="J60" t="n">
+        <v>-13.83</v>
+      </c>
+      <c r="K60" t="n">
+        <v>-22445.78</v>
+      </c>
+      <c r="L60" t="n">
+        <v>-66.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-24
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2651,6 +2651,46 @@
         <v>-66.03</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>01/24/2026</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>11873.3</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.2328945415145907</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.7671054584854093</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-186.79</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-25.41</v>
+      </c>
+      <c r="G61" t="n">
+        <v>-21683.68</v>
+      </c>
+      <c r="H61" t="n">
+        <v>-70.42</v>
+      </c>
+      <c r="I61" t="n">
+        <v>-437.62</v>
+      </c>
+      <c r="J61" t="n">
+        <v>-13.66</v>
+      </c>
+      <c r="K61" t="n">
+        <v>-22121.3</v>
+      </c>
+      <c r="L61" t="n">
+        <v>-65.06999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-25
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2691,6 +2691,46 @@
         <v>-65.06999999999999</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>01/25/2026</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>11840.99</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.2356344770773015</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.7643655229226985</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-190.24</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-25.88</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-21740.91</v>
+      </c>
+      <c r="H62" t="n">
+        <v>-70.61</v>
+      </c>
+      <c r="I62" t="n">
+        <v>-462.7</v>
+      </c>
+      <c r="J62" t="n">
+        <v>-14.22</v>
+      </c>
+      <c r="K62" t="n">
+        <v>-22203.61</v>
+      </c>
+      <c r="L62" t="n">
+        <v>-65.22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-26
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2731,6 +2731,46 @@
         <v>-65.22</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>01/26/2026</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>11536.27</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.2394848264837869</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.7605151735162131</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-206.93</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-28.15</v>
+      </c>
+      <c r="G63" t="n">
+        <v>-22018.25</v>
+      </c>
+      <c r="H63" t="n">
+        <v>-71.51000000000001</v>
+      </c>
+      <c r="I63" t="n">
+        <v>-490.09</v>
+      </c>
+      <c r="J63" t="n">
+        <v>-15.07</v>
+      </c>
+      <c r="K63" t="n">
+        <v>-22508.34</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-66.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-27
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2771,6 +2771,46 @@
         <v>-66.11</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>01/27/2026</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>11394.85</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.2427946360339521</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.7572053639660479</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-215.67</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-29.34</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-22163.52</v>
+      </c>
+      <c r="H64" t="n">
+        <v>-71.98</v>
+      </c>
+      <c r="I64" t="n">
+        <v>-486.24</v>
+      </c>
+      <c r="J64" t="n">
+        <v>-14.95</v>
+      </c>
+      <c r="K64" t="n">
+        <v>-22649.76</v>
+      </c>
+      <c r="L64" t="n">
+        <v>-66.53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-28
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2811,6 +2811,46 @@
         <v>-66.53</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>01/28/2026</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>11625.89</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.2434540290739574</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.7565459709260426</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-205.6</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-27.97</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-21996.24</v>
+      </c>
+      <c r="H65" t="n">
+        <v>-71.44</v>
+      </c>
+      <c r="I65" t="n">
+        <v>-422.48</v>
+      </c>
+      <c r="J65" t="n">
+        <v>-12.99</v>
+      </c>
+      <c r="K65" t="n">
+        <v>-22418.72</v>
+      </c>
+      <c r="L65" t="n">
+        <v>-65.84999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-29
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2851,6 +2851,46 @@
         <v>-65.84999999999999</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>01/29/2026</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>11269</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.2458624122915205</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.7541375877084795</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-223.49</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-30.41</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-22293.38</v>
+      </c>
+      <c r="H66" t="n">
+        <v>-72.40000000000001</v>
+      </c>
+      <c r="I66" t="n">
+        <v>-482.23</v>
+      </c>
+      <c r="J66" t="n">
+        <v>-14.82</v>
+      </c>
+      <c r="K66" t="n">
+        <v>-22775.61</v>
+      </c>
+      <c r="L66" t="n">
+        <v>-66.90000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-30
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2891,6 +2891,46 @@
         <v>-66.90000000000001</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>01/30/2026</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>10956.4</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.237431419224339</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.762568580775661</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-236.89</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-30.18</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-22486.75</v>
+      </c>
+      <c r="H67" t="n">
+        <v>-72.91</v>
+      </c>
+      <c r="I67" t="n">
+        <v>-651.45</v>
+      </c>
+      <c r="J67" t="n">
+        <v>-20.03</v>
+      </c>
+      <c r="K67" t="n">
+        <v>-23138.2</v>
+      </c>
+      <c r="L67" t="n">
+        <v>-67.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-01-31
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2931,6 +2931,46 @@
         <v>-67.86</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>01/31/2026</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>10417.61</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.249843725829219</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.750156274170781</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-272.32</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-34.69</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-23026.92</v>
+      </c>
+      <c r="H68" t="n">
+        <v>-74.66</v>
+      </c>
+      <c r="I68" t="n">
+        <v>-650.08</v>
+      </c>
+      <c r="J68" t="n">
+        <v>-19.98</v>
+      </c>
+      <c r="K68" t="n">
+        <v>-23677</v>
+      </c>
+      <c r="L68" t="n">
+        <v>-69.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-01
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2971,6 +2971,46 @@
         <v>-69.44</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>02/01/2026</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>9630.23</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.2613837494045819</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.7386162505954181</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-318.36</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-40.56</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-23728.71</v>
+      </c>
+      <c r="H69" t="n">
+        <v>-76.94</v>
+      </c>
+      <c r="I69" t="n">
+        <v>-785.66</v>
+      </c>
+      <c r="J69" t="n">
+        <v>-23.79</v>
+      </c>
+      <c r="K69" t="n">
+        <v>-24514.37</v>
+      </c>
+      <c r="L69" t="n">
+        <v>-71.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-02
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3011,6 +3011,46 @@
         <v>-71.8</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>02/02/2026</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>9441.6</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.2646812310596689</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.7353187689403311</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-329.55</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-41.98</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-23899.18</v>
+      </c>
+      <c r="H70" t="n">
+        <v>-77.48999999999999</v>
+      </c>
+      <c r="I70" t="n">
+        <v>-803.84</v>
+      </c>
+      <c r="J70" t="n">
+        <v>-24.34</v>
+      </c>
+      <c r="K70" t="n">
+        <v>-24703.02</v>
+      </c>
+      <c r="L70" t="n">
+        <v>-72.34999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-03
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3051,6 +3051,46 @@
         <v>-72.34999999999999</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>02/03/2026</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>9956.700000000001</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.2526948899720284</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.7473051100279716</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-296.87</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-37.82</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-23401.06</v>
+      </c>
+      <c r="H71" t="n">
+        <v>-75.87</v>
+      </c>
+      <c r="I71" t="n">
+        <v>-786.84</v>
+      </c>
+      <c r="J71" t="n">
+        <v>-23.82</v>
+      </c>
+      <c r="K71" t="n">
+        <v>-24187.9</v>
+      </c>
+      <c r="L71" t="n">
+        <v>-70.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-04
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3091,6 +3091,46 @@
         <v>-70.84</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>02/04/2026</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>9585.17</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.2546777055239792</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.7453222944760208</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-316.33</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-40.3</v>
+      </c>
+      <c r="G72" t="n">
+        <v>-23697.72</v>
+      </c>
+      <c r="H72" t="n">
+        <v>-76.84</v>
+      </c>
+      <c r="I72" t="n">
+        <v>-861.72</v>
+      </c>
+      <c r="J72" t="n">
+        <v>-26.09</v>
+      </c>
+      <c r="K72" t="n">
+        <v>-24559.44</v>
+      </c>
+      <c r="L72" t="n">
+        <v>-71.93000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-05
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3131,6 +3131,46 @@
         <v>-71.93000000000001</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>02/05/2026</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>8742.799999999999</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.2555396841306177</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.7444603158693823</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-358.01</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-45.61</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-24333.09</v>
+      </c>
+      <c r="H73" t="n">
+        <v>-78.90000000000001</v>
+      </c>
+      <c r="I73" t="n">
+        <v>-1068.72</v>
+      </c>
+      <c r="J73" t="n">
+        <v>-32.36</v>
+      </c>
+      <c r="K73" t="n">
+        <v>-25401.81</v>
+      </c>
+      <c r="L73" t="n">
+        <v>-74.39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-06
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3171,6 +3171,46 @@
         <v>-74.39</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>02/06/2026</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>8731.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.2450454044534087</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.7549545955465913</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-353.76</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-42.37</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-24299.87</v>
+      </c>
+      <c r="H74" t="n">
+        <v>-78.66</v>
+      </c>
+      <c r="I74" t="n">
+        <v>-1163.24</v>
+      </c>
+      <c r="J74" t="n">
+        <v>-35.22</v>
+      </c>
+      <c r="K74" t="n">
+        <v>-25463.11</v>
+      </c>
+      <c r="L74" t="n">
+        <v>-74.47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-07
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3211,6 +3211,46 @@
         <v>-74.47</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>02/07/2026</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>9279.24</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.2383866365551371</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.7616133634448629</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-319.06</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-38.21</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-23824.56</v>
+      </c>
+      <c r="H75" t="n">
+        <v>-77.12</v>
+      </c>
+      <c r="I75" t="n">
+        <v>-1090.8</v>
+      </c>
+      <c r="J75" t="n">
+        <v>-33.03</v>
+      </c>
+      <c r="K75" t="n">
+        <v>-24915.36</v>
+      </c>
+      <c r="L75" t="n">
+        <v>-72.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-08
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3251,6 +3251,46 @@
         <v>-72.86</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>02/08/2026</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>9764.35</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.2389734473272497</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.7610265526727503</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-292.51</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-35.03</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-23460.83</v>
+      </c>
+      <c r="H76" t="n">
+        <v>-75.95</v>
+      </c>
+      <c r="I76" t="n">
+        <v>-1019.43</v>
+      </c>
+      <c r="J76" t="n">
+        <v>-30.4</v>
+      </c>
+      <c r="K76" t="n">
+        <v>-24480.26</v>
+      </c>
+      <c r="L76" t="n">
+        <v>-71.48999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-09
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3291,6 +3291,46 @@
         <v>-71.48999999999999</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>02/09/2026</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>9365.299999999999</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.2422875806110708</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.7577124193889292</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-316.94</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-37.96</v>
+      </c>
+      <c r="G77" t="n">
+        <v>-23795.55</v>
+      </c>
+      <c r="H77" t="n">
+        <v>-77.03</v>
+      </c>
+      <c r="I77" t="n">
+        <v>-1083.75</v>
+      </c>
+      <c r="J77" t="n">
+        <v>-32.32</v>
+      </c>
+      <c r="K77" t="n">
+        <v>-24879.3</v>
+      </c>
+      <c r="L77" t="n">
+        <v>-72.65000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-10
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3331,6 +3331,46 @@
         <v>-72.65000000000001</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>02/10/2026</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>9118.940000000001</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.2470222779281854</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.7529777220718146</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-333.72</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-39.97</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-24025.4</v>
+      </c>
+      <c r="H78" t="n">
+        <v>-77.77</v>
+      </c>
+      <c r="I78" t="n">
+        <v>-1100.27</v>
+      </c>
+      <c r="J78" t="n">
+        <v>-32.82</v>
+      </c>
+      <c r="K78" t="n">
+        <v>-25125.67</v>
+      </c>
+      <c r="L78" t="n">
+        <v>-73.37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-11
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3371,6 +3371,46 @@
         <v>-73.37</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>02/11/2026</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>9231.27</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.237570868307493</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.762429131692507</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-321.18</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-38.46</v>
+      </c>
+      <c r="G79" t="n">
+        <v>-23853.57</v>
+      </c>
+      <c r="H79" t="n">
+        <v>-77.22</v>
+      </c>
+      <c r="I79" t="n">
+        <v>-1159.77</v>
+      </c>
+      <c r="J79" t="n">
+        <v>-34.59</v>
+      </c>
+      <c r="K79" t="n">
+        <v>-25013.34</v>
+      </c>
+      <c r="L79" t="n">
+        <v>-73.04000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-12
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3411,6 +3411,46 @@
         <v>-73.04000000000001</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>02/12/2026</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>9390.84</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.2372190378971422</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.7627809621028578</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-312.05</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-37.37</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-23728.61</v>
+      </c>
+      <c r="H80" t="n">
+        <v>-76.81</v>
+      </c>
+      <c r="I80" t="n">
+        <v>-1126.02</v>
+      </c>
+      <c r="J80" t="n">
+        <v>-33.58</v>
+      </c>
+      <c r="K80" t="n">
+        <v>-24853.77</v>
+      </c>
+      <c r="L80" t="n">
+        <v>-72.58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-13
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3451,6 +3451,46 @@
         <v>-72.58</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>02/13/2026</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>9191.639999999999</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.2394647885250994</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.7605352114749006</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-329.85</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-37.27</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-23951.19</v>
+      </c>
+      <c r="H81" t="n">
+        <v>-77.41</v>
+      </c>
+      <c r="I81" t="n">
+        <v>-1151.78</v>
+      </c>
+      <c r="J81" t="n">
+        <v>-34.35</v>
+      </c>
+      <c r="K81" t="n">
+        <v>-25102.97</v>
+      </c>
+      <c r="L81" t="n">
+        <v>-73.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-14
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3491,6 +3491,46 @@
         <v>-73.2</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>02/14/2026</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>9731</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.2354351560586131</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.7645648439413869</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-294.16</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-33.24</v>
+      </c>
+      <c r="G82" t="n">
+        <v>-23501.78</v>
+      </c>
+      <c r="H82" t="n">
+        <v>-75.95</v>
+      </c>
+      <c r="I82" t="n">
+        <v>-1061.83</v>
+      </c>
+      <c r="J82" t="n">
+        <v>-31.67</v>
+      </c>
+      <c r="K82" t="n">
+        <v>-24563.61</v>
+      </c>
+      <c r="L82" t="n">
+        <v>-71.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-15
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3531,6 +3531,46 @@
         <v>-71.63</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>02/15/2026</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>9598.16</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.242646236788244</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.757353763211756</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-307.72</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-34.77</v>
+      </c>
+      <c r="G83" t="n">
+        <v>-23672.56</v>
+      </c>
+      <c r="H83" t="n">
+        <v>-76.51000000000001</v>
+      </c>
+      <c r="I83" t="n">
+        <v>-1073.89</v>
+      </c>
+      <c r="J83" t="n">
+        <v>-31.56</v>
+      </c>
+      <c r="K83" t="n">
+        <v>-24746.45</v>
+      </c>
+      <c r="L83" t="n">
+        <v>-72.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-16
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3571,6 +3571,46 @@
         <v>-72.05</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>02/16/2026</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>9608.030000000001</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.2431908283538754</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.7568091716461246</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-307.54</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-34.75</v>
+      </c>
+      <c r="G84" t="n">
+        <v>-23670.31</v>
+      </c>
+      <c r="H84" t="n">
+        <v>-76.5</v>
+      </c>
+      <c r="I84" t="n">
+        <v>-1066.26</v>
+      </c>
+      <c r="J84" t="n">
+        <v>-31.33</v>
+      </c>
+      <c r="K84" t="n">
+        <v>-24736.57</v>
+      </c>
+      <c r="L84" t="n">
+        <v>-72.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-17
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3611,6 +3611,46 @@
         <v>-72.02</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>02/17/2026</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>9410.139999999999</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.2423188177825589</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.7576811822174411</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-318.78</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-36.02</v>
+      </c>
+      <c r="G85" t="n">
+        <v>-23811.87</v>
+      </c>
+      <c r="H85" t="n">
+        <v>-76.95999999999999</v>
+      </c>
+      <c r="I85" t="n">
+        <v>-1122.6</v>
+      </c>
+      <c r="J85" t="n">
+        <v>-32.99</v>
+      </c>
+      <c r="K85" t="n">
+        <v>-24934.47</v>
+      </c>
+      <c r="L85" t="n">
+        <v>-72.59999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-18
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3651,6 +3651,46 @@
         <v>-72.59999999999999</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>02/18/2026</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>9452.469999999999</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.2395311777718252</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.7604688222281748</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-314.14</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-35.5</v>
+      </c>
+      <c r="G86" t="n">
+        <v>-23753.45</v>
+      </c>
+      <c r="H86" t="n">
+        <v>-76.77</v>
+      </c>
+      <c r="I86" t="n">
+        <v>-1138.69</v>
+      </c>
+      <c r="J86" t="n">
+        <v>-33.46</v>
+      </c>
+      <c r="K86" t="n">
+        <v>-24892.14</v>
+      </c>
+      <c r="L86" t="n">
+        <v>-72.48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-19
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3691,6 +3691,46 @@
         <v>-72.48</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>02/19/2026</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>8992.99</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.2474013351478005</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.7525986648521995</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-347.51</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-39.27</v>
+      </c>
+      <c r="G87" t="n">
+        <v>-24173.65</v>
+      </c>
+      <c r="H87" t="n">
+        <v>-78.13</v>
+      </c>
+      <c r="I87" t="n">
+        <v>-1177.97</v>
+      </c>
+      <c r="J87" t="n">
+        <v>-34.62</v>
+      </c>
+      <c r="K87" t="n">
+        <v>-25351.62</v>
+      </c>
+      <c r="L87" t="n">
+        <v>-73.81999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-20
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3731,6 +3731,46 @@
         <v>-73.81999999999999</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>02/20/2026</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>9017.030000000001</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.2497591506634206</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.7502408493365794</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-353.1</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-37.76</v>
+      </c>
+      <c r="G88" t="n">
+        <v>-24226.81</v>
+      </c>
+      <c r="H88" t="n">
+        <v>-78.17</v>
+      </c>
+      <c r="I88" t="n">
+        <v>-1150.76</v>
+      </c>
+      <c r="J88" t="n">
+        <v>-33.82</v>
+      </c>
+      <c r="K88" t="n">
+        <v>-25377.57</v>
+      </c>
+      <c r="L88" t="n">
+        <v>-73.78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-21
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3771,6 +3771,46 @@
         <v>-73.78</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>02/21/2026</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>9374.48</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.2438417473332335</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.7561582526667665</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-325.26</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-34.79</v>
+      </c>
+      <c r="G89" t="n">
+        <v>-23903.16</v>
+      </c>
+      <c r="H89" t="n">
+        <v>-77.13</v>
+      </c>
+      <c r="I89" t="n">
+        <v>-1117.14</v>
+      </c>
+      <c r="J89" t="n">
+        <v>-32.83</v>
+      </c>
+      <c r="K89" t="n">
+        <v>-25020.12</v>
+      </c>
+      <c r="L89" t="n">
+        <v>-72.73999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-22
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3811,6 +3811,46 @@
         <v>-72.73999999999999</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>02/22/2026</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>9169.01</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.2538023500717298</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.7461976499282702</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-346.48</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-37.06</v>
+      </c>
+      <c r="G90" t="n">
+        <v>-24149.86</v>
+      </c>
+      <c r="H90" t="n">
+        <v>-77.92</v>
+      </c>
+      <c r="I90" t="n">
+        <v>-1125.73</v>
+      </c>
+      <c r="J90" t="n">
+        <v>-32.6</v>
+      </c>
+      <c r="K90" t="n">
+        <v>-25275.59</v>
+      </c>
+      <c r="L90" t="n">
+        <v>-73.38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-23
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3851,6 +3851,46 @@
         <v>-73.38</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>02/23/2026</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>9217.540000000001</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.2464356284593587</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.7535643715406413</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-337.53</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-36.1</v>
+      </c>
+      <c r="G91" t="n">
+        <v>-24045.75</v>
+      </c>
+      <c r="H91" t="n">
+        <v>-77.59</v>
+      </c>
+      <c r="I91" t="n">
+        <v>-1181.32</v>
+      </c>
+      <c r="J91" t="n">
+        <v>-34.21</v>
+      </c>
+      <c r="K91" t="n">
+        <v>-25227.07</v>
+      </c>
+      <c r="L91" t="n">
+        <v>-73.23999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-24
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3891,6 +3891,46 @@
         <v>-73.23999999999999</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>02/24/2026</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>8814.75</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.2451242745093181</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.7548757254906819</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-362.64</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-38.79</v>
+      </c>
+      <c r="G92" t="n">
+        <v>-24337.71</v>
+      </c>
+      <c r="H92" t="n">
+        <v>-78.53</v>
+      </c>
+      <c r="I92" t="n">
+        <v>-1292.14</v>
+      </c>
+      <c r="J92" t="n">
+        <v>-37.42</v>
+      </c>
+      <c r="K92" t="n">
+        <v>-25629.85</v>
+      </c>
+      <c r="L92" t="n">
+        <v>-74.41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-25
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3931,6 +3931,46 @@
         <v>-74.41</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>02/25/2026</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>9167.34</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0.2470002370263118</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.7529997629736882</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-341.23</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-36.5</v>
+      </c>
+      <c r="G93" t="n">
+        <v>-24088.75</v>
+      </c>
+      <c r="H93" t="n">
+        <v>-77.73</v>
+      </c>
+      <c r="I93" t="n">
+        <v>-1188.52</v>
+      </c>
+      <c r="J93" t="n">
+        <v>-34.42</v>
+      </c>
+      <c r="K93" t="n">
+        <v>-25277.27</v>
+      </c>
+      <c r="L93" t="n">
+        <v>-73.39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-26
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3971,6 +3971,46 @@
         <v>-73.39</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>02/26/2026</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>9766.27</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.2387191444856278</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.7612808555143722</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-295.48</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-31.6</v>
+      </c>
+      <c r="G94" t="n">
+        <v>-23556.88</v>
+      </c>
+      <c r="H94" t="n">
+        <v>-76.01000000000001</v>
+      </c>
+      <c r="I94" t="n">
+        <v>-1121.45</v>
+      </c>
+      <c r="J94" t="n">
+        <v>-32.48</v>
+      </c>
+      <c r="K94" t="n">
+        <v>-24678.33</v>
+      </c>
+      <c r="L94" t="n">
+        <v>-71.65000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-27
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4011,6 +4011,46 @@
         <v>-71.65000000000001</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>02/27/2026</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>9228.780000000001</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0.2451365678766332</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.7548634321233668</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-342.25</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-34.75</v>
+      </c>
+      <c r="G95" t="n">
+        <v>-24075.29</v>
+      </c>
+      <c r="H95" t="n">
+        <v>-77.56</v>
+      </c>
+      <c r="I95" t="n">
+        <v>-1190.54</v>
+      </c>
+      <c r="J95" t="n">
+        <v>-34.48</v>
+      </c>
+      <c r="K95" t="n">
+        <v>-25265.83</v>
+      </c>
+      <c r="L95" t="n">
+        <v>-73.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update profit files after running on 2026-02-28
</commit_message>
<xml_diff>
--- a/data/profit_data.xlsx
+++ b/data/profit_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4051,6 +4051,46 @@
         <v>-73.25</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>02/28/2026</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>8743.440000000001</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0.2504107866633722</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.7495892133366278</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-380.3</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-38.61</v>
+      </c>
+      <c r="G96" t="n">
+        <v>-24487.77</v>
+      </c>
+      <c r="H96" t="n">
+        <v>-78.89</v>
+      </c>
+      <c r="I96" t="n">
+        <v>-1263.4</v>
+      </c>
+      <c r="J96" t="n">
+        <v>-36.59</v>
+      </c>
+      <c r="K96" t="n">
+        <v>-25751.17</v>
+      </c>
+      <c r="L96" t="n">
+        <v>-74.65000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>